<commit_message>
still getting singlwe page data
</commit_message>
<xml_diff>
--- a/ExtractData.xlsx
+++ b/ExtractData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amitc\Documents\UiPath\Web Scrapingbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062E78EA-FE18-468A-946C-EBA02F6F3C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC757EE-72DB-45D1-BC77-628EE2C7832A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2595" yWindow="2595" windowWidth="21600" windowHeight="11835" xr2:uid="{31679DB8-20F4-4541-B16F-25A8D2C40E98}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Description</t>
   </si>
@@ -42,106 +42,100 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Apple iPhone 12 (128GB) - Blue</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_aps_sr_pg1_1?ie=UTF8&amp;adId=A0289169I1H125BE6KZA&amp;url=%2FNew-Apple-iPhone-12-128GB%2Fdp%2FB08L5TNJHG%2Fref%3Dsr_1_1_sspa%3Fcrid%3D2RANQ33UCZBYG%26keywords%3Diphone%2B12%26qid%3D1641892183%26sprefix%3Diphone%2B12%252Caps%252C446%26sr%3D8-1-spons%26psc%3D1&amp;qualifier=1641892183&amp;id=4679358428108533&amp;widgetName=sp_atf</t>
-  </si>
-  <si>
-    <t>Apple iPhone 12 Mini (128GB) - Green</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_aps_sr_pg1_1?ie=UTF8&amp;adId=A028769726XR1HVZVN0D2&amp;url=%2FNew-Apple-iPhone-Mini-128GB%2Fdp%2FB08L5VQTG9%2Fref%3Dsr_1_2_sspa%3Fcrid%3D2RANQ33UCZBYG%26keywords%3Diphone%2B12%26qid%3D1641892183%26sprefix%3Diphone%2B12%252Caps%252C446%26sr%3D8-2-spons%26psc%3D1&amp;qualifier=1641892183&amp;id=4679358428108533&amp;widgetName=sp_atf</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-12-128GB/dp/B08L5TNJHG/ref=sr_1_3?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-3</t>
-  </si>
-  <si>
-    <t>Apple iPhone 12 (64GB) - Green</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-12-64GB/dp/B08L5W16HX/ref=sr_1_4?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-4</t>
-  </si>
-  <si>
-    <t>Apple iPhone 12 (64GB) - Blue</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-12-64GB/dp/B08L5WHFT9/ref=sr_1_5?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-5</t>
-  </si>
-  <si>
-    <t>Apple iPhone 12 (64GB) - (Product) RED</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-12-64GB/dp/B08L5TGWD1/ref=sr_1_6?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-6</t>
-  </si>
-  <si>
-    <t>Apple iPhone 13 (128GB) - Pink</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/Apple-iPhone-13-128GB-Pink/dp/B09G9FPGTN/ref=sr_1_7?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-7</t>
-  </si>
-  <si>
-    <t>Apple iPhone 12 (64GB) - Purple</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-12-64GB/dp/B0932QYBH8/ref=sr_1_8?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-8</t>
-  </si>
-  <si>
-    <t>Apple iPhone 12 Mini (64GB) - Purple</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-Mini-64GB/dp/B0932PTZ5V/ref=sr_1_9?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-9</t>
-  </si>
-  <si>
-    <t>New Apple iPhone 12 (64GB) - Blue with Apple 20W USB-C Power Adapter</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-12-64GB/dp/B08Z6N9ZF3/ref=sr_1_10?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-10</t>
-  </si>
-  <si>
-    <t>New Apple iPhone 12 (64GB) - (Product) RED with Apple 20W USB-C Power Adapter</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-12-64GB/dp/B08Z73MPX8/ref=sr_1_11?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-11</t>
-  </si>
-  <si>
-    <t>New Apple iPhone 12 (64GB) - Green with Apple 20W USB-C Power Adapter</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-12-64GB/dp/B08Z6YKWCM/ref=sr_1_12?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-12</t>
-  </si>
-  <si>
-    <t>Apple iPhone 12 Mini (128GB) - Black</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-Mini-128GB/dp/B08L5VG843/ref=sr_1_13?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-13</t>
-  </si>
-  <si>
-    <t>New Apple iPhone 12 Mini (128GB) - Black with Apple 20W USB-C Power Adapter</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-Mini-128GB/dp/B08Z6SCHXH/ref=sr_1_14?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-14</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-Mini-128GB/dp/B08L5VQTG9/ref=sr_1_15?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-15</t>
-  </si>
-  <si>
-    <t>Apple iPhone 12 Mini (128GB) - (Product) RED</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-Mini-128GB/dp/B08L5WH99K/ref=sr_1_16?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-16</t>
-  </si>
-  <si>
-    <t>New Apple iPhone 12 (128GB) - Blue with Apple 20W USB-C Power Adapter</t>
-  </si>
-  <si>
-    <t>https://www.amazon.in/New-Apple-iPhone-12-128GB/dp/B08Z6QNWK8/ref=sr_1_17?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-17</t>
-  </si>
-  <si>
     <t>New Apple iPhone 12 Mini (128GB) - Green with Apple 20W USB-C Power Adapter</t>
   </si>
   <si>
     <t>https://www.amazon.in/New-Apple-iPhone-Mini-128GB/dp/B08Z72HXHT/ref=sr_1_18?crid=2RANQ33UCZBYG&amp;keywords=iphone+12&amp;qid=1641892183&amp;sprefix=iphone+12%2Caps%2C446&amp;sr=8-18</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A03s (Black, 4GB RAM, 64GB Storage) with No Cost EMI/Additional Exchange Offers</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Samsung-Galaxy-Storage-Additional-Exchange/dp/B09C8FWW2H/ref=sr_1_297?crid=AJ35DUY62ZJ0&amp;keywords=iphone+12&amp;qid=1641908990&amp;sprefix=ipho%2Caps%2C595&amp;sr=8-297</t>
+  </si>
+  <si>
+    <t>Nillkin Case for OnePlus 9R One Plus 9R (1+9) R (6.55" Inch) Super Frosted Hard Back Cover PC Black Color</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Nillkin-OnePlus-Super-Frosted-Cover/dp/B094QHHWQF/ref=sr_1_298?crid=AJ35DUY62ZJ0&amp;keywords=iphone+12&amp;qid=1641908990&amp;sprefix=ipho%2Caps%2C595&amp;sr=8-298</t>
+  </si>
+  <si>
+    <t>itel A23 Pro Jio (Lake Blue, 1GB RAM, 8 GB Storage, 5'' Bright Display) (L5006C)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/itel-Storage-Bright-Display-L5006C/dp/B08T7G9HFM/ref=sr_1_299?crid=AJ35DUY62ZJ0&amp;keywords=iphone+12&amp;qid=1641908990&amp;sprefix=ipho%2Caps%2C595&amp;sr=8-299</t>
+  </si>
+  <si>
+    <t>(Renewed) Dell Inspiron 5501 Laptop|i5-1035G1|8GB DDR4|512GB SSD|Win 10 HSL|NVIDIA MX330 2GB|15.6" FHD|Backlit|Silver</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Renewed-Dell-Inspiron-i5-1035G1-Backlit/dp/B091SJFHMP/ref=sr_1_291?keywords=dell+laptop+i5&amp;qid=1641909341&amp;sprefix=dell+laptop%2Caps%2C394&amp;sr=8-291</t>
+  </si>
+  <si>
+    <t>(Renewed) Dell Intel Core i5-4th Gen 14 Inch (35.56 cms) 1366x768 HD Laptop (16GB RAM/128GB SSD &amp; 1TB HDD/Windows 10 Pro/MS Office/Intel Integrated HD Graphics 4600/2.1Kg,Silver) Latitude E6440</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Dell-1366x768-Integrated-Graphics-Latitude/dp/B099YLCD7W/ref=sr_1_292?keywords=dell+laptop+i5&amp;qid=1641909341&amp;sprefix=dell+laptop%2Caps%2C394&amp;sr=8-292</t>
+  </si>
+  <si>
+    <t>(Renewed) Dell Latitude Laptop E5480 Intel Core i5 7th Gen. - 7300u Processor, 16 GB Ram &amp; 2TB GB SSD, 14.1 Inches Full HD Screen Notebook Computer</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Renewed-Dell-Latitude-Laptop-E5480/dp/B091N2WV24/ref=sr_1_293?keywords=dell+laptop+i5&amp;qid=1641909341&amp;sprefix=dell+laptop%2Caps%2C394&amp;sr=8-293</t>
+  </si>
+  <si>
+    <t>Dell Latitude 3510 Intel Core i3-10110U /4GB/1TB/UBUNTU/ 39.62 cm (15.6 INCH )Screen/1 Year Warranty</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Dell-Latitude-3510-i3-10110U-Warranty/dp/B08B9X82C6/ref=sr_1_289?keywords=dell+laptop+i5&amp;qid=1641909341&amp;sprefix=dell+laptop%2Caps%2C394&amp;sr=8-289</t>
+  </si>
+  <si>
+    <t>(Renewed) Dell Latitude E6440-i5-16 GB-320 GB 14-inch Laptop (4th Gen Core i5/16GB/320GB/Windows 10/Integrated Graphics), Silver</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Dell-E6440-i5-16-GB-320-GB-Integrated/dp/B07LB4NZYL/ref=sr_1_290?keywords=dell+laptop+i5&amp;qid=1641909341&amp;sprefix=dell+laptop%2Caps%2C394&amp;sr=8-290</t>
+  </si>
+  <si>
+    <t>(Renewed) Dell Latitude Laptop E7480 Intel Core i5 - 7200U Processor 7th Gen, 16 GB Ram &amp; 2TB SSD, 14.1 Inches Touch Screen (Ultra Slim &amp; Light 1.58KG) Notebook Computer</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Renewed-Dell-Latitude-Laptop-E7480/dp/B092S94YCP/ref=sr_1_291?keywords=dell+laptop+i5&amp;qid=1641909341&amp;sprefix=dell+laptop%2Caps%2C394&amp;sr=8-291</t>
+  </si>
+  <si>
+    <t>(Renewed) Dell Latitude Laptop E7480 Intel Core i5 - 7200U Processor 7th Gen, 32 GB Ram &amp; 256 GB SSD, 14.1 Inches Touch Screen (Ultra Slim &amp; Light 1.58KG) Notebook Computer</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Renewed-Dell-Latitude-Laptop-E7480/dp/B092S8GGRG/ref=sr_1_292?keywords=dell+laptop+i5&amp;qid=1641909341&amp;sprefix=dell+laptop%2Caps%2C394&amp;sr=8-292</t>
+  </si>
+  <si>
+    <t>(Renewed) Dell Intel Core i5-4th Gen 14 Inch(35.56 cms) 1366x768 HD Laptop (8GB RAM/256GB SSD/Windows 10 Pro/MS Office/Intel Integrated HD Graphics 4400/1.9Kg,Silver) Latitude E7440</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Dell-1366x768-Integrated-Graphics-Latitude/dp/B09B52F871/ref=sr_1_295?keywords=dell+laptop+i5&amp;qid=1641909341&amp;sprefix=dell+laptop%2Caps%2C394&amp;sr=8-295</t>
+  </si>
+  <si>
+    <t>(Renewed) Dell Latitude E6420-i5-4 GB-512 GB 14-inch Laptop (2nd Gen Core i5/4GB//Windows 7/Integrated Graphics), Greyish Silver</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Dell-E6420-i5-4-GB-512-GB-Integrated/dp/B07LB4XT5T/ref=sr_1_296?keywords=dell+laptop+i5&amp;qid=1641909341&amp;sprefix=dell+laptop%2Caps%2C394&amp;sr=8-296</t>
+  </si>
+  <si>
+    <t>(Renewed) Dell Latitude E5270 Laptop (CORE I5 6TH GEN/4GB/500GB/WEBCAM/12.5'' NO TOUCH/Windows 10 Home)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Renewed-Dell-Latitude-E5270-Windows/dp/B08XVV5BLP/ref=sr_1_297?keywords=dell+laptop+i5&amp;qid=1641909341&amp;sprefix=dell+laptop%2Caps%2C394&amp;sr=8-297</t>
+  </si>
+  <si>
+    <t>Dell Latitude 3490 8th Gen Intel Core i5-8250U 14 inches HD LED Business Laptop (4GB/1TB/Windows 10 Home Single Language/2 GB AMD Radeon Graphics, Black, 1.72 kg)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Latitude-3490-i5-8250U-Language-Graphics/dp/B07PXLPWQM/ref=sr_1_298?keywords=dell+laptop+i5&amp;qid=1641909341&amp;sprefix=dell+laptop%2Caps%2C394&amp;sr=8-298</t>
+  </si>
+  <si>
+    <t>(Renewed) Dell Intel Core i5 6th Gen 14-Inch(35.56 cms) 1366 x 768 HD Laptop (32GB RAM /1TB HDD/Windows 10 Pro/MS Office/Intel HD Integrated Graphics/ Black/1.5Kg,Black) Latitude E5480</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Dell-Integrated-Graphics-Latitude-E5480/dp/B09M4271RP/ref=sr_1_299?keywords=dell+laptop+i5&amp;qid=1641909341&amp;sprefix=dell+laptop%2Caps%2C394&amp;sr=8-299</t>
   </si>
 </sst>
 </file>
@@ -509,146 +503,130 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>